<commit_message>
added momentum, batch and anneannealing
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -54,7 +54,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +64,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -152,11 +158,11 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -509,7 +515,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4">
         <v>33970</v>
       </c>
@@ -538,7 +544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4">
         <v>33971</v>
       </c>
@@ -567,7 +573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4">
         <v>33972</v>
       </c>
@@ -596,7 +602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4">
         <v>33973</v>
       </c>
@@ -625,7 +631,7 @@
         <v>61.6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4">
         <v>33974</v>
       </c>
@@ -654,7 +660,7 @@
         <v>111.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4">
         <v>33975</v>
       </c>
@@ -683,7 +689,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4">
         <v>33976</v>
       </c>
@@ -712,7 +718,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4">
         <v>33977</v>
       </c>
@@ -741,7 +747,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4">
         <v>33978</v>
       </c>
@@ -770,7 +776,7 @@
         <v>104.8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4">
         <v>33979</v>
       </c>
@@ -799,7 +805,7 @@
         <v>136.8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4">
         <v>33980</v>
       </c>
@@ -828,7 +834,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4">
         <v>33981</v>
       </c>
@@ -857,7 +863,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4">
         <v>33982</v>
       </c>
@@ -886,7 +892,7 @@
         <v>118</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4">
         <v>33983</v>
       </c>
@@ -915,7 +921,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="4">
         <v>33984</v>
       </c>
@@ -944,7 +950,7 @@
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="4">
         <v>33985</v>
       </c>
@@ -973,7 +979,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="4">
         <v>33986</v>
       </c>
@@ -1002,7 +1008,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="4">
         <v>33987</v>
       </c>
@@ -1031,7 +1037,7 @@
         <v>103.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="4">
         <v>33988</v>
       </c>

</xml_diff>